<commit_message>
updated test cases and data processor
</commit_message>
<xml_diff>
--- a/data_processing/dimension_play_log.xlsx
+++ b/data_processing/dimension_play_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anieuwsma/Library/Mobile Documents/com~apple~CloudDocs/repositories/dimension/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A449C793-1B65-E149-9E0C-88F4C86128EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCB827F-09D5-0642-B675-8F992A09C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33420" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>"QUANTITY-2-B", "NOTTOP-O", "TOUCH-K-K", "TOUCH-B-W", "NOTOUCH-O-K", "RATIO-4-G-K"</t>
-  </si>
-  <si>
     <t>Andrew</t>
   </si>
   <si>
@@ -106,27 +103,15 @@
     <t>"NOTOUCH-G-G", "TOUCH-G-W", "TOUCH-G-K", "NOTOUCH-K-W", "RATIO-4-O-B", "RATIO-4-B-G"</t>
   </si>
   <si>
-    <t>"QUANTITY-1-K", "QUANTITY-1-B", "NOTTOP-K", "TOUCH-K-W", "NOTOUCH-K-B", "GT-K-B"</t>
-  </si>
-  <si>
     <t>"QUANTITY-1-W", "QUANTITY-2-O", "NOTOUCH-G-K", "NOTOUCH-O-B", "NOTOUCH-O-W", "GT-B-W"</t>
   </si>
   <si>
-    <t>"NOTTOP-G", "NOTTOP-O", "NOTOUCH-K-K", "TOUCH-G-B", "TOUCH-O-B", "GT-W-G"</t>
-  </si>
-  <si>
     <t>"QUANTITY-1-G", "QUANTITY-1-O", "NOTOUCH-G-B", "NOTOUCH-G-W", "NOTOUCH-B-W", "RATIO-4-K-W"</t>
   </si>
   <si>
-    <t>"QUANTITY-2-G", "QUANTITY-2-B", "TOP-W", "NOTTOP-G", "NOTTOP-W", "NOTOUCH-O-O"</t>
-  </si>
-  <si>
     <t>"TOP-K", "TOP-B", "TOUCH-G-G", "TOUCH-B-B", "NOTOUCH-B-B", "GT-G-O"</t>
   </si>
   <si>
-    <t>"NOTTOP-B", "TOUCH-O-O", "TOUCH-W-W", "TOUCH-O-K", "TOUCH-K-B", "GT-O-K"</t>
-  </si>
-  <si>
     <t>"QUANTITY-2-W", "NOTOUCH-W-W", "TOUCH-G-O", "TOUCH-O-W", "NOTOUCH-G-O", "RATIO-4-W-O"</t>
   </si>
   <si>
@@ -136,9 +121,6 @@
     <t>"QUANTITY-1-K", "QUANTITY-1-B", "TOUCH-W-W", "NOTOUCH-K-K", "TOUCH-K-W", "NOTOUCH-K-B"</t>
   </si>
   <si>
-    <t>"TOP-O", "NOTTOP-O", "NOTTOP-K", "TOUCH-B-W", "NOTOUCH-K-W", "GT-K-B"</t>
-  </si>
-  <si>
     <t>"QUANTITY-2-B", "TOUCH-G-G", "TOUCH-B-B", "NOTOUCH-O-K", "RATIO-4-K-W", "GT-G-O"</t>
   </si>
   <si>
@@ -148,16 +130,34 @@
     <t>"QUANTITY-1-W", "QUANTITY-2-O", "TOUCH-B-B", "NOTOUCH-G-W", "NOTOUCH-G-K", "NOTOUCH-O-W"</t>
   </si>
   <si>
-    <t>"QUANTITY-1-G", "QUANTITY-2-G", "NOTTOP-B", "NOTOUCH-W-W", "TOUCH-G-B", "NOTOUCH-G-B"</t>
-  </si>
-  <si>
     <t>"QUANTITY-1-O", "TOUCH-O-W", "TOUCH-O-K", "NOTOUCH-O-K", "NOTOUCH-B-W", "RATIO-4-W-O"</t>
   </si>
   <si>
-    <t>"NOTTOP-G", "NOTTOP-W", "NOTOUCH-O-O", "TOUCH-G-O", "TOUCH-G-K", "TOUCH-O-B"</t>
-  </si>
-  <si>
-    <t>"QUANTITY-2-W", "NOTTOP-K", "NOTTOP-W", "NOTTOP-B", "RATIO-4-O-B", "RATIO-4-B-G"</t>
+    <t>"QUANTITY-2-B", "BOTTOM-O", "TOUCH-K-K", "TOUCH-B-W", "NOTOUCH-O-K", "RATIO-4-G-K"</t>
+  </si>
+  <si>
+    <t>"QUANTITY-1-K", "QUANTITY-1-B", "BOTTOM-K", "TOUCH-K-W", "NOTOUCH-K-B", "GT-K-B"</t>
+  </si>
+  <si>
+    <t>"BOTTOM-G", "BOTTOM-O", "NOTOUCH-K-K", "TOUCH-G-B", "TOUCH-O-B", "GT-W-G"</t>
+  </si>
+  <si>
+    <t>"QUANTITY-2-G", "QUANTITY-2-B", "TOP-W", "BOTTOM-G", "BOTTOM-W", "NOTOUCH-O-O"</t>
+  </si>
+  <si>
+    <t>"BOTTOM-B", "TOUCH-O-O", "TOUCH-W-W", "TOUCH-O-K", "TOUCH-K-B", "GT-O-K"</t>
+  </si>
+  <si>
+    <t>"TOP-O", "BOTTOM-O", "BOTTOM-K", "TOUCH-B-W", "NOTOUCH-K-W", "GT-K-B"</t>
+  </si>
+  <si>
+    <t>"QUANTITY-1-G", "QUANTITY-2-G", "BOTTOM-B", "NOTOUCH-W-W", "TOUCH-G-B", "NOTOUCH-G-B"</t>
+  </si>
+  <si>
+    <t>"BOTTOM-G", "BOTTOM-W", "NOTOUCH-O-O", "TOUCH-G-O", "TOUCH-G-K", "TOUCH-O-B"</t>
+  </si>
+  <si>
+    <t>"QUANTITY-2-W", "BOTTOM-K", "BOTTOM-W", "BOTTOM-B", "RATIO-4-O-B", "RATIO-4-B-G"</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -655,10 +655,10 @@
         <v>45162.561974386575</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>19</v>
@@ -747,10 +747,10 @@
         <v>45162.571911018516</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -789,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>23</v>
@@ -836,10 +836,10 @@
         <v>45162.576029942131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>22</v>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>22</v>
@@ -928,10 +928,10 @@
         <v>45162.579697303241</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>20</v>
@@ -1014,10 +1014,10 @@
         <v>45162.585219560184</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>23</v>
@@ -1103,10 +1103,10 @@
         <v>45162.590993055557</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>20</v>
@@ -1180,10 +1180,10 @@
         <v>45162.59478407407</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
@@ -1222,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>23</v>
@@ -1263,10 +1263,10 @@
         <v>45162.599410601848</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -1305,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>21</v>
@@ -1349,10 +1349,10 @@
         <v>45162.644606620372</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
@@ -1394,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>22</v>
@@ -1438,10 +1438,10 @@
         <v>45162.647342141208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
@@ -1480,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>22</v>
@@ -1524,10 +1524,10 @@
         <v>45162.650415763885</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -1569,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>20</v>
@@ -1613,10 +1613,10 @@
         <v>45162.652708182868</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>22</v>
@@ -1705,10 +1705,10 @@
         <v>45162.654775104165</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>23</v>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>22</v>
@@ -1791,10 +1791,10 @@
         <v>45162.656472650458</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>19</v>
@@ -1880,10 +1880,10 @@
         <v>45162.658933460647</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>20</v>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>19</v>
@@ -1954,10 +1954,10 @@
         <v>45162.660345717595</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>21</v>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>21</v>
@@ -2025,10 +2025,10 @@
         <v>45162.66273142361</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>20</v>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>21</v>
@@ -2117,10 +2117,10 @@
         <v>45162.664630601852</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>20</v>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>21</v>
@@ -2203,7 +2203,7 @@
         <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -2245,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>21</v>
@@ -2292,7 +2292,7 @@
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>21</v>

</xml_diff>